<commit_message>
Updated figures and data
</commit_message>
<xml_diff>
--- a/data/question1_summary.xlsx
+++ b/data/question1_summary.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\Projects\Uncertainty Survey\uncertainty_survey\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{D922616D-FE39-44E7-A8C9-8EF941281FAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF1F2BC4-CAF0-447F-B963-0B7DB1A072C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="15255" windowHeight="14700" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="question1_summary" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>CODE</t>
   </si>
@@ -91,9 +104,6 @@
     <t>SUCCESS_CRITERIA</t>
   </si>
   <si>
-    <t>INFORMATION</t>
-  </si>
-  <si>
     <t>PREDICTION</t>
   </si>
   <si>
@@ -134,12 +144,18 @@
   </si>
   <si>
     <t>OTHER</t>
+  </si>
+  <si>
+    <t>EVIDENCE_ACTION</t>
+  </si>
+  <si>
+    <t>*I split methods into two</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -276,7 +292,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -459,6 +475,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -623,9 +657,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -980,16 +1018,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F56"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A53" sqref="A53:F55"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1223,27 +1262,27 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="A16" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B16" s="1">
+      <c r="B16" s="3">
         <v>14</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>15</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="3">
         <v>9</v>
       </c>
-      <c r="E16" s="1">
+      <c r="E16" s="3">
         <v>12</v>
       </c>
-      <c r="F16" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
+      <c r="F16" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B19" s="1">
@@ -1262,88 +1301,91 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="1">
+      <c r="B20" s="3">
         <v>25</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="3">
         <v>22</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="3">
         <v>24</v>
       </c>
-      <c r="E20" s="1">
+      <c r="E20" s="3">
         <v>12</v>
       </c>
-      <c r="F20" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="F20" s="3">
+        <v>4</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="1">
+      <c r="B21" s="3">
         <v>3</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="3">
         <v>3</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="3">
         <v>8</v>
       </c>
-      <c r="E21" s="1">
+      <c r="E21" s="3">
         <v>3</v>
       </c>
-      <c r="F21" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+      <c r="F21" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="1">
-        <v>1</v>
-      </c>
-      <c r="C22" s="1">
-        <v>2</v>
-      </c>
-      <c r="D22" s="1">
-        <v>1</v>
-      </c>
-      <c r="E22" s="1">
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
+      <c r="E22" s="3">
         <v>0</v>
       </c>
-      <c r="F22" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="F22" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="1">
+      <c r="B23" s="3">
         <v>5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="3">
         <v>7</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E23" s="1">
+      <c r="E23" s="3">
         <v>0</v>
       </c>
-      <c r="F23" s="1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
+      <c r="F23" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B24" s="1">
@@ -1361,9 +1403,15 @@
       <c r="F24" s="1">
         <v>4</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="s">
+      <c r="H24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="4" t="s">
         <v>21</v>
       </c>
       <c r="B25" s="1">
@@ -1382,378 +1430,376 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+    <row r="26" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="1">
-        <v>1</v>
-      </c>
-      <c r="C26" s="1">
-        <v>2</v>
-      </c>
-      <c r="D26" s="1">
-        <v>4</v>
-      </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="1">
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>2</v>
+      </c>
+      <c r="D27" s="1">
+        <v>4</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B27">
-        <v>45</v>
-      </c>
-      <c r="C27">
-        <v>51</v>
-      </c>
-      <c r="D27">
-        <v>55</v>
-      </c>
-      <c r="E27">
-        <v>28</v>
-      </c>
-      <c r="F27">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B29" s="1">
+      <c r="B31" s="1">
         <v>8</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C31" s="1">
         <v>16</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D31" s="1">
         <v>15</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E31" s="1">
         <v>7</v>
       </c>
-      <c r="F29" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="1">
-        <v>5</v>
-      </c>
-      <c r="C32" s="1">
-        <v>8</v>
-      </c>
-      <c r="D32" s="1">
-        <v>5</v>
-      </c>
-      <c r="E32" s="1">
-        <v>10</v>
-      </c>
-      <c r="F32" s="1">
-        <v>5</v>
+      <c r="F31" s="1">
+        <v>4</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B34" s="1">
+        <v>5</v>
+      </c>
+      <c r="C34" s="1">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1">
+        <v>5</v>
+      </c>
+      <c r="E34" s="1">
+        <v>10</v>
+      </c>
+      <c r="F34" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B36" s="1">
+        <v>8</v>
+      </c>
+      <c r="C36" s="1">
+        <v>6</v>
+      </c>
+      <c r="D36" s="1">
+        <v>6</v>
+      </c>
+      <c r="E36" s="1">
+        <v>4</v>
+      </c>
+      <c r="F36" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="1">
-        <v>8</v>
-      </c>
-      <c r="C34" s="1">
-        <v>6</v>
-      </c>
-      <c r="D34" s="1">
-        <v>6</v>
-      </c>
-      <c r="E34" s="1">
-        <v>4</v>
-      </c>
-      <c r="F34" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>27</v>
-      </c>
-      <c r="B38">
+      <c r="B40">
         <v>17</v>
       </c>
-      <c r="C38">
+      <c r="C40">
         <v>10</v>
       </c>
-      <c r="D38">
+      <c r="D40">
         <v>5</v>
       </c>
-      <c r="E38">
+      <c r="E40">
         <v>5</v>
       </c>
-      <c r="F38">
+      <c r="F40">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B41" s="1">
-        <v>33</v>
-      </c>
-      <c r="C41" s="1">
-        <v>21</v>
-      </c>
-      <c r="D41" s="1">
-        <v>14</v>
-      </c>
-      <c r="E41" s="1">
-        <v>6</v>
-      </c>
-      <c r="F41" s="1">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="B43" s="1">
-        <v>2</v>
-      </c>
-      <c r="C43" s="1">
-        <v>4</v>
-      </c>
-      <c r="D43" s="1">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1</v>
+      </c>
+      <c r="C42" s="2">
+        <v>4</v>
+      </c>
+      <c r="D42" s="2">
         <v>3</v>
       </c>
-      <c r="E43" s="1">
+      <c r="E42" s="2">
         <v>0</v>
       </c>
-      <c r="F43" s="1">
+      <c r="F42" s="2">
         <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B44" s="1">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="C44" s="1">
+        <v>21</v>
+      </c>
+      <c r="D44" s="1">
+        <v>14</v>
+      </c>
+      <c r="E44" s="1">
+        <v>6</v>
+      </c>
+      <c r="F44" s="1">
         <v>5</v>
-      </c>
-      <c r="D44" s="1">
-        <v>1</v>
-      </c>
-      <c r="E44" s="1">
-        <v>1</v>
-      </c>
-      <c r="F44" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="1">
-        <v>10</v>
-      </c>
-      <c r="C45" s="1">
-        <v>14</v>
-      </c>
-      <c r="D45" s="1">
-        <v>17</v>
-      </c>
-      <c r="E45" s="1">
-        <v>7</v>
-      </c>
-      <c r="F45" s="1">
-        <v>7</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B46" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C46" s="1">
         <v>4</v>
       </c>
       <c r="D46" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E46" s="1">
+        <v>0</v>
+      </c>
+      <c r="F46" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B47" s="1">
+        <v>3</v>
+      </c>
+      <c r="C47" s="1">
         <v>5</v>
       </c>
-      <c r="F46" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47">
-        <v>19</v>
-      </c>
-      <c r="C47">
-        <v>27</v>
-      </c>
-      <c r="D47">
-        <v>27</v>
-      </c>
-      <c r="E47">
-        <v>13</v>
-      </c>
-      <c r="F47">
-        <v>13</v>
+      <c r="D47" s="1">
+        <v>1</v>
+      </c>
+      <c r="E47" s="1">
+        <v>1</v>
+      </c>
+      <c r="F47" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B48" s="1">
+        <v>10</v>
+      </c>
+      <c r="C48" s="1">
+        <v>14</v>
+      </c>
+      <c r="D48" s="1">
+        <v>17</v>
+      </c>
+      <c r="E48" s="1">
+        <v>7</v>
+      </c>
+      <c r="F48" s="1">
+        <v>7</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B49" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C49" s="1">
         <v>4</v>
       </c>
       <c r="D49" s="1">
+        <v>6</v>
+      </c>
+      <c r="E49" s="1">
         <v>5</v>
       </c>
-      <c r="E49" s="1">
-        <v>1</v>
-      </c>
       <c r="F49" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A50" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B50" s="1">
-        <v>11</v>
-      </c>
-      <c r="C50" s="1">
+      <c r="B50">
+        <v>19</v>
+      </c>
+      <c r="C50">
+        <v>27</v>
+      </c>
+      <c r="D50">
+        <v>27</v>
+      </c>
+      <c r="E50">
         <v>13</v>
       </c>
-      <c r="D50" s="1">
+      <c r="F50">
         <v>13</v>
       </c>
-      <c r="E50" s="1">
-        <v>10</v>
-      </c>
-      <c r="F50" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B51">
-        <v>13</v>
-      </c>
-      <c r="C51">
-        <v>17</v>
-      </c>
-      <c r="D51">
-        <v>18</v>
-      </c>
-      <c r="E51">
-        <v>11</v>
-      </c>
-      <c r="F51">
-        <v>6</v>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B52" s="1">
+        <v>2</v>
+      </c>
+      <c r="C52" s="1">
+        <v>4</v>
+      </c>
+      <c r="D52" s="1">
+        <v>5</v>
+      </c>
+      <c r="E52" s="1">
+        <v>1</v>
+      </c>
+      <c r="F52" s="1">
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B53" s="1">
+        <v>11</v>
+      </c>
+      <c r="C53" s="1">
+        <v>13</v>
+      </c>
+      <c r="D53" s="1">
+        <v>13</v>
+      </c>
+      <c r="E53" s="1">
+        <v>10</v>
+      </c>
+      <c r="F53" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B54">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>17</v>
+      </c>
+      <c r="D54">
+        <v>18</v>
+      </c>
+      <c r="E54">
+        <v>11</v>
+      </c>
+      <c r="F54">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B56" s="2">
         <v>0</v>
       </c>
-      <c r="C53" s="1">
-        <v>1</v>
-      </c>
-      <c r="D53" s="1">
-        <v>2</v>
-      </c>
-      <c r="E53" s="1">
+      <c r="C56" s="2">
+        <v>1</v>
+      </c>
+      <c r="D56" s="2">
+        <v>2</v>
+      </c>
+      <c r="E56" s="2">
         <v>3</v>
       </c>
-      <c r="F53" s="1">
+      <c r="F56" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A54" s="1" t="s">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="2"/>
+      <c r="B57" s="2"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B54" s="1">
-        <v>1</v>
-      </c>
-      <c r="C54" s="1">
-        <v>4</v>
-      </c>
-      <c r="D54" s="1">
+      <c r="B58" s="1">
+        <v>2</v>
+      </c>
+      <c r="C58" s="1">
+        <v>7</v>
+      </c>
+      <c r="D58" s="1">
+        <v>10</v>
+      </c>
+      <c r="E58" s="1">
+        <v>7</v>
+      </c>
+      <c r="F58" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59">
         <v>3</v>
       </c>
-      <c r="E54" s="1">
-        <v>0</v>
-      </c>
-      <c r="F54" s="1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A55" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B55" s="1">
-        <v>2</v>
-      </c>
-      <c r="C55" s="1">
-        <v>7</v>
-      </c>
-      <c r="D55" s="1">
+      <c r="C59">
+        <v>12</v>
+      </c>
+      <c r="D59">
+        <v>15</v>
+      </c>
+      <c r="E59">
         <v>10</v>
       </c>
-      <c r="E55" s="1">
-        <v>7</v>
-      </c>
-      <c r="F55" s="1">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B56">
-        <v>3</v>
-      </c>
-      <c r="C56">
-        <v>12</v>
-      </c>
-      <c r="D56">
-        <v>15</v>
-      </c>
-      <c r="E56">
-        <v>10</v>
-      </c>
-      <c r="F56">
+      <c r="F59">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>